<commit_message>
uploading Lab 2 files
</commit_message>
<xml_diff>
--- a/Lab 1/Data.xlsx
+++ b/Lab 1/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\2 CCE\Term 6\2027\DataStructure\Main Lab Repo\Lab 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D57E62E-533B-4C08-9E6B-F22D7F122599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D7206E-2410-45C0-A0B4-BA490EC0D2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D9DA8AEB-F847-47CF-8BB9-65079700BD3D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Array size</t>
   </si>
@@ -48,6 +48,21 @@
   </si>
   <si>
     <t>Selection Sort</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>Quick S</t>
+  </si>
+  <si>
+    <t>Merge S</t>
+  </si>
+  <si>
+    <t>Heap S.</t>
   </si>
 </sst>
 </file>
@@ -84,12 +99,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -120,6 +141,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -198,9 +228,9 @@
   <autoFilter ref="A1:D11" xr:uid="{C56A4834-02F1-4FA4-9383-B4D7DA8A7DCC}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{5D046DD8-52D5-4F69-9E6E-D9DB889D7573}" name="Array size" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{EAA8F334-BCE4-4F0D-9AC4-8277EC1F4B6E}" name="Bubble Sort" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{E3CC450E-4FA5-4904-9B98-598F4F050FC6}" name="Insertion Sort" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{47FAD97B-853B-4AB7-9C75-20F2634F8BC4}" name="Selection Sort" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{EAA8F334-BCE4-4F0D-9AC4-8277EC1F4B6E}" name="Bubble Sort" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{E3CC450E-4FA5-4904-9B98-598F4F050FC6}" name="Insertion Sort" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{47FAD97B-853B-4AB7-9C75-20F2634F8BC4}" name="Selection Sort" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -523,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC183902-0986-408D-86FB-036E51694E46}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,7 +567,7 @@
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>50</v>
       </c>
@@ -566,7 +596,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>100</v>
       </c>
@@ -581,7 +611,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>500</v>
       </c>
@@ -596,7 +626,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1000</v>
       </c>
@@ -611,7 +641,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5000</v>
       </c>
@@ -626,7 +656,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>10000</v>
       </c>
@@ -641,7 +671,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>50000</v>
       </c>
@@ -656,7 +686,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>100000</v>
       </c>
@@ -672,7 +702,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>150000</v>
       </c>
@@ -687,7 +717,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>250000</v>
       </c>
@@ -702,34 +732,240 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>50</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>100</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>500</v>
+      </c>
+      <c r="B17" s="6">
+        <v>6.3</v>
+      </c>
+      <c r="C17" s="6">
+        <v>3.2</v>
+      </c>
+      <c r="D17" s="6">
+        <v>3</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>1000</v>
+      </c>
+      <c r="B18" s="6">
+        <v>32.130000000000003</v>
+      </c>
+      <c r="C18" s="6">
+        <v>13.52</v>
+      </c>
+      <c r="D18" s="6">
+        <v>13</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1.01</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1.02</v>
+      </c>
+      <c r="G18" s="6">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <v>5000</v>
+      </c>
+      <c r="B19" s="6">
+        <v>778.71</v>
+      </c>
+      <c r="C19" s="6">
+        <v>348.76</v>
+      </c>
+      <c r="D19" s="6">
+        <v>323.16000000000003</v>
+      </c>
+      <c r="E19" s="6">
+        <v>7.1</v>
+      </c>
+      <c r="F19" s="6">
+        <v>7</v>
+      </c>
+      <c r="G19" s="6">
+        <v>11.14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <v>10000</v>
+      </c>
+      <c r="B20" s="6">
+        <v>3249.78</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1319.78</v>
+      </c>
+      <c r="D20" s="6">
+        <v>1252.3800000000001</v>
+      </c>
+      <c r="E20" s="6">
+        <v>12.27</v>
+      </c>
+      <c r="F20" s="6">
+        <v>14.61</v>
+      </c>
+      <c r="G20" s="6">
+        <v>21.61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
+        <v>50000</v>
+      </c>
+      <c r="B21" s="6">
+        <v>82193.009999999995</v>
+      </c>
+      <c r="C21" s="6">
+        <v>33936.97</v>
+      </c>
+      <c r="D21" s="6">
+        <v>33050.449999999997</v>
+      </c>
+      <c r="E21" s="6">
+        <v>72.11</v>
+      </c>
+      <c r="F21" s="6">
+        <v>84.18</v>
+      </c>
+      <c r="G21" s="6">
+        <v>130.78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>100000</v>
+      </c>
+      <c r="B22" s="6">
+        <v>338244.59</v>
+      </c>
+      <c r="C22" s="6">
+        <v>150274.49</v>
+      </c>
+      <c r="D22" s="6">
+        <v>137543.03</v>
+      </c>
+      <c r="E22" s="6">
+        <v>173.95</v>
+      </c>
+      <c r="F22" s="6">
+        <v>172.97</v>
+      </c>
+      <c r="G22" s="6">
+        <v>294.93</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -740,12 +976,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -899,15 +1132,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A5177AF-DCC9-4799-960D-94993B1B7E93}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08A0274C-F25F-44D2-BD58-FCA8222F3184}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -931,10 +1168,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08A0274C-F25F-44D2-BD58-FCA8222F3184}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A5177AF-DCC9-4799-960D-94993B1B7E93}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>